<commit_message>
[AOS] View All 구현
</commit_message>
<xml_diff>
--- a/Localization/LangPack_EverydayJapanese.xlsx
+++ b/Localization/LangPack_EverydayJapanese.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimkihoon/Work/Project/EverydayJapanese/Localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5DE155-FC94-FB45-96C4-367875E2693C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30361095-49D9-644B-A45C-B20755101A7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="760" windowWidth="33600" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="33600" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -893,24 +893,6 @@
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Inconsolata"/>
     </font>
   </fonts>
   <fills count="5">
@@ -966,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -988,9 +970,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2181,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F246"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="273" zoomScaleNormal="273" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="136" zoomScaleNormal="273" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2772,506 +2751,506 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="6"/>
+      <c r="A49" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="1" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="1" t="s">
-        <v>108</v>
+        <v>145</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="11" t="s">
-        <v>145</v>
+      <c r="A54" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="B54" s="6"/>
-      <c r="C54" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>153</v>
+      <c r="C54" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="11" t="s">
-        <v>146</v>
+      <c r="A55" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="B55" s="6"/>
-      <c r="C55" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>154</v>
+      <c r="C55" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="11" t="s">
-        <v>147</v>
+      <c r="A56" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="B56" s="6"/>
-      <c r="C56" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>155</v>
+      <c r="C56" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="11" t="s">
-        <v>148</v>
+      <c r="A57" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B57" s="6"/>
-      <c r="C57" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>156</v>
+      <c r="C57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="11" t="s">
-        <v>149</v>
+      <c r="A58" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B58" s="6"/>
-      <c r="C58" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>157</v>
+      <c r="C58" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="11" t="s">
-        <v>150</v>
+      <c r="A59" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="B59" s="6"/>
-      <c r="C59" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>158</v>
+      <c r="C59" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="11" t="s">
-        <v>151</v>
+      <c r="A60" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B60" s="6"/>
-      <c r="C60" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="11" t="s">
+      <c r="C60" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="D60" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="16">
+      <c r="A61" s="6" t="s">
+        <v>163</v>
+      </c>
       <c r="B61" s="6"/>
-      <c r="C61" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>160</v>
+      <c r="C61" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="16">
       <c r="A62" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="16">
       <c r="A63" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="16">
       <c r="A64" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="16">
-      <c r="A65" s="6" t="s">
-        <v>168</v>
-      </c>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="6"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
+      <c r="A66" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="10"/>
+      <c r="A67" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>180</v>
+      <c r="A68" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="12" t="s">
+      <c r="A69" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12" t="s">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D69" s="1" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="16">
+      <c r="A70" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="16">
       <c r="A71" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="16">
-      <c r="A72" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="B72" s="6"/>
-      <c r="C72" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>191</v>
+      <c r="C72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="13" t="s">
-        <v>227</v>
+      <c r="A73" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B73" s="6"/>
-      <c r="C73" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>195</v>
+      <c r="C73" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="13" t="s">
-        <v>196</v>
+      <c r="A74" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="B74" s="6"/>
-      <c r="C74" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>197</v>
+      <c r="C74" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="13" t="s">
-        <v>198</v>
+      <c r="A75" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="B75" s="6"/>
-      <c r="C75" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>199</v>
+      <c r="C75" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="13" t="s">
-        <v>238</v>
+      <c r="A76" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="B76" s="6"/>
-      <c r="C76" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>201</v>
+      <c r="C76" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="13" t="s">
-        <v>239</v>
+      <c r="A77" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="B77" s="6"/>
-      <c r="C77" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>203</v>
+      <c r="C77" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="13" t="s">
-        <v>240</v>
+      <c r="A78" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="B78" s="6"/>
-      <c r="C78" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>205</v>
+      <c r="C78" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="13" t="s">
-        <v>241</v>
+      <c r="A79" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="B79" s="6"/>
-      <c r="C79" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>207</v>
+      <c r="C79" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="13" t="s">
-        <v>242</v>
+      <c r="A80" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="B80" s="6"/>
-      <c r="C80" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>209</v>
+      <c r="C80" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="13" t="s">
-        <v>243</v>
+      <c r="A81" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="B81" s="6"/>
-      <c r="C81" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>211</v>
+      <c r="C81" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="13" t="s">
-        <v>228</v>
+      <c r="A82" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="B82" s="6"/>
-      <c r="C82" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>213</v>
+      <c r="C82" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="13" t="s">
-        <v>229</v>
+      <c r="A83" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="B83" s="6"/>
-      <c r="C83" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>214</v>
+      <c r="C83" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="13" t="s">
-        <v>230</v>
+      <c r="A84" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="B84" s="6"/>
-      <c r="C84" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>215</v>
+      <c r="C84" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="13" t="s">
-        <v>231</v>
+      <c r="A85" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="B85" s="6"/>
-      <c r="C85" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>216</v>
+      <c r="C85" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="13" t="s">
-        <v>232</v>
+      <c r="A86" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="B86" s="6"/>
-      <c r="C86" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>217</v>
+      <c r="C86" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="13" t="s">
-        <v>233</v>
+      <c r="A87" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="B87" s="6"/>
-      <c r="C87" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>218</v>
+      <c r="C87" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="13" t="s">
-        <v>234</v>
+      <c r="A88" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="B88" s="6"/>
-      <c r="C88" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>220</v>
+      <c r="C88" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="13" t="s">
-        <v>235</v>
+      <c r="A89" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="B89" s="6"/>
-      <c r="C89" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>222</v>
+      <c r="C89" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="13" t="s">
-        <v>236</v>
+      <c r="A90" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="B90" s="6"/>
-      <c r="C90" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>224</v>
+      <c r="C90" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="13" t="s">
-        <v>237</v>
-      </c>
+      <c r="A91" s="6"/>
       <c r="B91" s="6"/>
-      <c r="C91" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>226</v>
-      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="6"/>
@@ -4196,12 +4175,6 @@
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
       <c r="D245" s="6"/>
-    </row>
-    <row r="246" spans="1:4">
-      <c r="A246" s="6"/>
-      <c r="B246" s="6"/>
-      <c r="C246" s="6"/>
-      <c r="D246" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>